<commit_message>
added generailised excel utility file
</commit_message>
<xml_diff>
--- a/testData/LoginData.xlsx
+++ b/testData/LoginData.xlsx
@@ -27,12 +27,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>emailAddress</t>
   </si>
   <si>
-    <t>Password</t>
+    <t>password</t>
   </si>
   <si>
     <t>test@gmail.com</t>
@@ -42,6 +42,9 @@
   </si>
   <si>
     <t>soxiy51987@icousd.com</t>
+  </si>
+  <si>
+    <t>Password</t>
   </si>
 </sst>
 </file>
@@ -54,7 +57,7 @@
     <numFmt numFmtId="178" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="179" formatCode="_ &quot;₹&quot;* #,##0_ ;_ &quot;₹&quot;* \-#,##0_ ;_ &quot;₹&quot;* &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
-  <fonts count="22">
+  <fonts count="21">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -74,13 +77,6 @@
       <color rgb="FF0000FF"/>
       <name val="Calibri"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -523,148 +519,148 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="176" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="179" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -998,7 +994,7 @@
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelRow="2" outlineLevelCol="1"/>
@@ -1028,7 +1024,7 @@
         <v>4</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>